<commit_message>
ajustes na descrição da matriz de citacao e no resumo21
</commit_message>
<xml_diff>
--- a/Experiment01_Resumo/Resumo_Exp01_V2.xlsx
+++ b/Experiment01_Resumo/Resumo_Exp01_V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Erica\hybrid_strategy_old\Experiment01_Resumo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Erica\hybrid_strategy\Experiment01_Resumo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="589">
   <si>
     <t>Database search</t>
   </si>
@@ -2623,7 +2623,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3203,6 +3203,27 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3254,30 +3275,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3293,6 +3290,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3302,6 +3308,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3310,6 +3331,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3371,32 +3401,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3722,12 +3731,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209217992"/>
-        <c:axId val="209222304"/>
+        <c:axId val="210849216"/>
+        <c:axId val="210846864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209217992"/>
+        <c:axId val="210849216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,7 +3829,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209222304"/>
+        <c:crossAx val="210846864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3828,7 +3837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209222304"/>
+        <c:axId val="210846864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3879,7 +3888,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209217992"/>
+        <c:crossAx val="210849216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4121,6 +4130,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4191,8 +4201,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209477816"/>
-        <c:axId val="209478208"/>
+        <c:axId val="211602992"/>
+        <c:axId val="211603384"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -4362,7 +4372,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209477816"/>
+        <c:axId val="211602992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4394,6 +4404,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4460,7 +4471,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209478208"/>
+        <c:crossAx val="211603384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4468,7 +4479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209478208"/>
+        <c:axId val="211603384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4514,6 +4525,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4547,7 +4559,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209477816"/>
+        <c:crossAx val="211602992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4561,6 +4573,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4772,6 +4785,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4859,12 +4873,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209219560"/>
-        <c:axId val="209221128"/>
+        <c:axId val="210843336"/>
+        <c:axId val="210850392"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209219560"/>
+        <c:axId val="210843336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4893,6 +4907,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4953,7 +4968,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209221128"/>
+        <c:crossAx val="210850392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4961,7 +4976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209221128"/>
+        <c:axId val="210850392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4990,6 +5005,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5044,7 +5060,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209219560"/>
+        <c:crossAx val="210843336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5058,6 +5074,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5242,6 +5259,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5329,12 +5347,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209216816"/>
-        <c:axId val="209218384"/>
+        <c:axId val="210846472"/>
+        <c:axId val="210845688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209216816"/>
+        <c:axId val="210846472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5363,6 +5381,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5423,7 +5442,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209218384"/>
+        <c:crossAx val="210845688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5431,7 +5450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209218384"/>
+        <c:axId val="210845688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5460,6 +5479,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5514,7 +5534,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209216816"/>
+        <c:crossAx val="210846472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5528,6 +5548,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6302,12 +6323,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209221520"/>
-        <c:axId val="209216032"/>
+        <c:axId val="210843728"/>
+        <c:axId val="210845296"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209221520"/>
+        <c:axId val="210843728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6347,7 +6368,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209216032"/>
+        <c:crossAx val="210845296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6355,7 +6376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209216032"/>
+        <c:axId val="210845296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6403,7 +6424,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209221520"/>
+        <c:crossAx val="210843728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6777,12 +6798,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209472720"/>
-        <c:axId val="209473112"/>
+        <c:axId val="211602208"/>
+        <c:axId val="211600248"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209472720"/>
+        <c:axId val="211602208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6875,7 +6896,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209473112"/>
+        <c:crossAx val="211600248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6883,7 +6904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209473112"/>
+        <c:axId val="211600248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6934,7 +6955,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209472720"/>
+        <c:crossAx val="211602208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7245,12 +7266,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209479776"/>
-        <c:axId val="209475856"/>
+        <c:axId val="211601424"/>
+        <c:axId val="211599072"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209479776"/>
+        <c:axId val="211601424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7340,7 +7361,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209475856"/>
+        <c:crossAx val="211599072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7348,7 +7369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209475856"/>
+        <c:axId val="211599072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7432,7 +7453,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209479776"/>
+        <c:crossAx val="211601424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7719,12 +7740,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="209473896"/>
-        <c:axId val="209475072"/>
+        <c:axId val="211595936"/>
+        <c:axId val="211599464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209473896"/>
+        <c:axId val="211595936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7814,7 +7835,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209475072"/>
+        <c:crossAx val="211599464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7822,7 +7843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209475072"/>
+        <c:axId val="211599464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7906,7 +7927,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209473896"/>
+        <c:crossAx val="211595936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8695,12 +8716,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209472328"/>
-        <c:axId val="209476248"/>
+        <c:axId val="211597504"/>
+        <c:axId val="211599856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209472328"/>
+        <c:axId val="211597504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8740,7 +8761,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209476248"/>
+        <c:crossAx val="211599856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8748,7 +8769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209476248"/>
+        <c:axId val="211599856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8796,7 +8817,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209472328"/>
+        <c:crossAx val="211597504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9035,6 +9056,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9105,8 +9127,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="209476640"/>
-        <c:axId val="209478992"/>
+        <c:axId val="211597896"/>
+        <c:axId val="211601032"/>
         <c:axId val="0"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -9276,7 +9298,7 @@
         </c:extLst>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="209476640"/>
+        <c:axId val="211597896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9308,6 +9330,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9374,7 +9397,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209478992"/>
+        <c:crossAx val="211601032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9382,7 +9405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209478992"/>
+        <c:axId val="211601032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9428,6 +9451,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9461,7 +9485,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209476640"/>
+        <c:crossAx val="211597896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9475,6 +9499,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14882,15 +14907,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>70377</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>49211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>8467</xdr:rowOff>
+      <xdr:colOff>339726</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15339,8 +15364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15350,22 +15375,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="221" t="s">
+      <c r="A1" s="228" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="222"/>
+      <c r="B1" s="229"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="230" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="224"/>
+      <c r="B2" s="231"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="223" t="s">
+      <c r="A3" s="230" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="224"/>
+      <c r="B3" s="231"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -15400,10 +15425,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="225" t="s">
+      <c r="A8" s="232" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="226"/>
+      <c r="B8" s="233"/>
     </row>
     <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -15473,7 +15498,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15488,18 +15513,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="279" t="s">
         <v>464</v>
       </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
-      <c r="F1" s="269"/>
-      <c r="G1" s="269"/>
-      <c r="H1" s="269"/>
-      <c r="I1" s="269"/>
-      <c r="J1" s="269"/>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="169" t="s">
@@ -16344,15 +16369,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="270" t="s">
+      <c r="A1" s="280" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="270"/>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="270"/>
-      <c r="G1" s="270"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
+      <c r="E1" s="280"/>
+      <c r="F1" s="280"/>
+      <c r="G1" s="280"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16366,7 +16391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
@@ -16387,19 +16412,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="243" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="236"/>
-      <c r="K1" s="236"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="243"/>
+      <c r="I1" s="243"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="243"/>
     </row>
     <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -17121,10 +17146,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="281" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="272"/>
+      <c r="B1" s="282"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="78" t="s">
@@ -17175,7 +17200,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17193,21 +17218,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="276" t="s">
+      <c r="A1" s="286" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="276"/>
-      <c r="C1" s="276"/>
-      <c r="D1" s="276"/>
-      <c r="E1" s="276"/>
-      <c r="F1" s="276"/>
-      <c r="G1" s="276"/>
-      <c r="H1" s="276"/>
-      <c r="I1" s="276"/>
-      <c r="J1" s="276"/>
-      <c r="K1" s="276"/>
-      <c r="L1" s="276"/>
-      <c r="M1" s="276"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
     </row>
     <row r="2" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="138" t="s">
@@ -17983,15 +18008,15 @@
     </row>
     <row r="26" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="131"/>
-      <c r="B26" s="273" t="s">
+      <c r="B26" s="283" t="s">
         <v>334</v>
       </c>
-      <c r="C26" s="274"/>
-      <c r="D26" s="274"/>
-      <c r="E26" s="274"/>
-      <c r="F26" s="274"/>
-      <c r="G26" s="274"/>
-      <c r="H26" s="275"/>
+      <c r="C26" s="284"/>
+      <c r="D26" s="284"/>
+      <c r="E26" s="284"/>
+      <c r="F26" s="284"/>
+      <c r="G26" s="284"/>
+      <c r="H26" s="285"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="66"/>
@@ -18159,10 +18184,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="238" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="239"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -18195,16 +18220,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="227" t="s">
+      <c r="A6" s="234" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="228"/>
+      <c r="B6" s="235"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="229" t="s">
+      <c r="A7" s="236" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="230"/>
+      <c r="B7" s="237"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -18286,16 +18311,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="240" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="234"/>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="235"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="242"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
@@ -18651,7 +18676,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18665,14 +18690,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="243" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="236"/>
-      <c r="C1" s="236"/>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -19134,7 +19159,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="140" t="s">
         <v>125</v>
       </c>
@@ -19158,7 +19183,7 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19186,27 +19211,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="244" t="s">
         <v>569</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="237"/>
-      <c r="I1" s="237"/>
-      <c r="J1" s="237"/>
-      <c r="K1" s="237"/>
-      <c r="L1" s="237"/>
-      <c r="M1" s="237"/>
-      <c r="N1" s="237"/>
-      <c r="O1" s="237"/>
-      <c r="P1" s="237"/>
-      <c r="Q1" s="237"/>
-      <c r="R1" s="237"/>
-      <c r="S1" s="237"/>
+      <c r="B1" s="244"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
+      <c r="G1" s="244"/>
+      <c r="H1" s="244"/>
+      <c r="I1" s="244"/>
+      <c r="J1" s="244"/>
+      <c r="K1" s="244"/>
+      <c r="L1" s="244"/>
+      <c r="M1" s="244"/>
+      <c r="N1" s="244"/>
+      <c r="O1" s="244"/>
+      <c r="P1" s="244"/>
+      <c r="Q1" s="244"/>
+      <c r="R1" s="244"/>
+      <c r="S1" s="244"/>
     </row>
     <row r="2" spans="1:22" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -21872,8 +21897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21883,49 +21908,49 @@
     <col min="3" max="3" width="21.85546875" style="87" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="87" customWidth="1"/>
     <col min="5" max="6" width="21.85546875" style="87" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" style="87" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="87" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" style="87" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="87"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="248" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
-      <c r="I1" s="250"/>
+      <c r="B1" s="249"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="238" t="s">
+      <c r="A2" s="250" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="238"/>
-      <c r="I2" s="238"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="250"/>
     </row>
     <row r="3" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="243" t="s">
+      <c r="A3" s="251" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="243"/>
-      <c r="C3" s="243"/>
-      <c r="D3" s="243"/>
-      <c r="E3" s="243"/>
-      <c r="F3" s="243"/>
-      <c r="G3" s="243"/>
-      <c r="H3" s="243"/>
-      <c r="I3" s="243"/>
+      <c r="B3" s="251"/>
+      <c r="C3" s="251"/>
+      <c r="D3" s="251"/>
+      <c r="E3" s="251"/>
+      <c r="F3" s="251"/>
+      <c r="G3" s="251"/>
+      <c r="H3" s="251"/>
+      <c r="I3" s="251"/>
       <c r="J3" s="70"/>
       <c r="K3" s="70"/>
       <c r="L3" s="70"/>
@@ -21938,12 +21963,12 @@
       <c r="S3" s="70"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="244" t="s">
+      <c r="A4" s="252" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="244"/>
+      <c r="B4" s="252"/>
+      <c r="C4" s="252"/>
+      <c r="D4" s="252"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="207" t="s">
@@ -21969,7 +21994,7 @@
       <c r="C6" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="251" t="s">
+      <c r="D6" s="253" t="s">
         <v>339</v>
       </c>
       <c r="E6" s="87" t="e">
@@ -21988,7 +22013,7 @@
       <c r="C7" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="D7" s="252"/>
+      <c r="D7" s="254"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="94" t="s">
@@ -22000,7 +22025,7 @@
       <c r="C8" s="91" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="252"/>
+      <c r="D8" s="254"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="94" t="s">
@@ -22012,7 +22037,7 @@
       <c r="C9" s="91" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="252"/>
+      <c r="D9" s="254"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="94" t="s">
@@ -22024,7 +22049,7 @@
       <c r="C10" s="91" t="s">
         <v>237</v>
       </c>
-      <c r="D10" s="252"/>
+      <c r="D10" s="254"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="94" t="s">
@@ -22036,7 +22061,7 @@
       <c r="C11" s="91" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="252"/>
+      <c r="D11" s="254"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="94" t="s">
@@ -22048,7 +22073,7 @@
       <c r="C12" s="91" t="s">
         <v>266</v>
       </c>
-      <c r="D12" s="252"/>
+      <c r="D12" s="254"/>
     </row>
     <row r="13" spans="1:19" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="141" t="s">
@@ -22060,7 +22085,7 @@
       <c r="C13" s="206" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="253"/>
+      <c r="D13" s="255"/>
     </row>
     <row r="14" spans="1:19" s="76" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="142" t="s">
@@ -22077,30 +22102,30 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="238" t="s">
+      <c r="A15" s="250" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
-      <c r="E15" s="238"/>
-      <c r="F15" s="238"/>
-      <c r="G15" s="238"/>
-      <c r="H15" s="238"/>
-      <c r="I15" s="238"/>
+      <c r="B15" s="250"/>
+      <c r="C15" s="250"/>
+      <c r="D15" s="250"/>
+      <c r="E15" s="250"/>
+      <c r="F15" s="250"/>
+      <c r="G15" s="250"/>
+      <c r="H15" s="250"/>
+      <c r="I15" s="250"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="243" t="s">
+      <c r="A16" s="251" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="243"/>
-      <c r="C16" s="243"/>
-      <c r="D16" s="243"/>
-      <c r="E16" s="243"/>
-      <c r="F16" s="243"/>
-      <c r="G16" s="243"/>
-      <c r="H16" s="243"/>
-      <c r="I16" s="243"/>
+      <c r="B16" s="251"/>
+      <c r="C16" s="251"/>
+      <c r="D16" s="251"/>
+      <c r="E16" s="251"/>
+      <c r="F16" s="251"/>
+      <c r="G16" s="251"/>
+      <c r="H16" s="251"/>
+      <c r="I16" s="251"/>
       <c r="J16" s="70"/>
       <c r="K16" s="70"/>
       <c r="L16" s="70"/>
@@ -22113,14 +22138,15 @@
       <c r="S16" s="70"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="244" t="s">
+      <c r="A17" s="287" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="244"/>
-      <c r="C17" s="244"/>
-      <c r="D17" s="244"/>
-      <c r="E17" s="244"/>
-      <c r="F17" s="244"/>
+      <c r="B17" s="288"/>
+      <c r="C17" s="288"/>
+      <c r="D17" s="288"/>
+      <c r="E17" s="288"/>
+      <c r="F17" s="288"/>
+      <c r="G17" s="288"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="207" t="s">
@@ -22141,6 +22167,9 @@
       <c r="F18" s="207" t="s">
         <v>201</v>
       </c>
+      <c r="G18" s="221" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="85" t="s">
@@ -22287,30 +22316,30 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="238" t="s">
+      <c r="A25" s="250" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="238"/>
-      <c r="C25" s="238"/>
-      <c r="D25" s="238"/>
-      <c r="E25" s="238"/>
-      <c r="F25" s="238"/>
-      <c r="G25" s="238"/>
-      <c r="H25" s="238"/>
-      <c r="I25" s="238"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
     </row>
     <row r="26" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="243" t="s">
+      <c r="A26" s="251" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="243"/>
-      <c r="C26" s="243"/>
-      <c r="D26" s="243"/>
-      <c r="E26" s="243"/>
-      <c r="F26" s="243"/>
-      <c r="G26" s="243"/>
-      <c r="H26" s="243"/>
-      <c r="I26" s="243"/>
+      <c r="B26" s="251"/>
+      <c r="C26" s="251"/>
+      <c r="D26" s="251"/>
+      <c r="E26" s="251"/>
+      <c r="F26" s="251"/>
+      <c r="G26" s="251"/>
+      <c r="H26" s="251"/>
+      <c r="I26" s="251"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="207" t="s">
@@ -22322,12 +22351,12 @@
       <c r="C27" s="207" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="245" t="s">
+      <c r="D27" s="256" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="245"/>
-      <c r="F27" s="245"/>
-      <c r="G27" s="245"/>
+      <c r="E27" s="256"/>
+      <c r="F27" s="256"/>
+      <c r="G27" s="256"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="92" t="s">
@@ -22339,12 +22368,12 @@
       <c r="C28" s="71">
         <v>0.59</v>
       </c>
-      <c r="D28" s="246" t="s">
+      <c r="D28" s="245" t="s">
         <v>285</v>
       </c>
-      <c r="E28" s="247"/>
-      <c r="F28" s="247"/>
-      <c r="G28" s="248"/>
+      <c r="E28" s="246"/>
+      <c r="F28" s="246"/>
+      <c r="G28" s="247"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="92" t="s">
@@ -22356,12 +22385,12 @@
       <c r="C29" s="71">
         <v>0.77</v>
       </c>
-      <c r="D29" s="240" t="s">
+      <c r="D29" s="258" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="241"/>
-      <c r="F29" s="241"/>
-      <c r="G29" s="242"/>
+      <c r="E29" s="259"/>
+      <c r="F29" s="259"/>
+      <c r="G29" s="260"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="92" t="s">
@@ -22373,12 +22402,12 @@
       <c r="C30" s="71">
         <v>0.41</v>
       </c>
-      <c r="D30" s="240" t="s">
+      <c r="D30" s="258" t="s">
         <v>287</v>
       </c>
-      <c r="E30" s="241"/>
-      <c r="F30" s="241"/>
-      <c r="G30" s="242"/>
+      <c r="E30" s="259"/>
+      <c r="F30" s="259"/>
+      <c r="G30" s="260"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="92" t="s">
@@ -22390,12 +22419,12 @@
       <c r="C31" s="71">
         <v>0.59</v>
       </c>
-      <c r="D31" s="240" t="s">
+      <c r="D31" s="258" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="241"/>
-      <c r="F31" s="241"/>
-      <c r="G31" s="242"/>
+      <c r="E31" s="259"/>
+      <c r="F31" s="259"/>
+      <c r="G31" s="260"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="92" t="s">
@@ -22407,12 +22436,12 @@
       <c r="C32" s="71">
         <v>0.5</v>
       </c>
-      <c r="D32" s="240" t="s">
+      <c r="D32" s="258" t="s">
         <v>288</v>
       </c>
-      <c r="E32" s="241"/>
-      <c r="F32" s="241"/>
-      <c r="G32" s="242"/>
+      <c r="E32" s="259"/>
+      <c r="F32" s="259"/>
+      <c r="G32" s="260"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="92" t="s">
@@ -22424,12 +22453,12 @@
       <c r="C33" s="71">
         <v>0.59</v>
       </c>
-      <c r="D33" s="240" t="s">
+      <c r="D33" s="258" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="241"/>
-      <c r="F33" s="241"/>
-      <c r="G33" s="242"/>
+      <c r="E33" s="259"/>
+      <c r="F33" s="259"/>
+      <c r="G33" s="260"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="92" t="s">
@@ -22441,25 +22470,25 @@
       <c r="C34" s="71">
         <v>0.54</v>
       </c>
-      <c r="D34" s="240" t="s">
+      <c r="D34" s="258" t="s">
         <v>291</v>
       </c>
-      <c r="E34" s="241"/>
-      <c r="F34" s="241"/>
-      <c r="G34" s="242"/>
+      <c r="E34" s="259"/>
+      <c r="F34" s="259"/>
+      <c r="G34" s="260"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="238" t="s">
+      <c r="A36" s="250" t="s">
         <v>315</v>
       </c>
-      <c r="B36" s="238"/>
-      <c r="C36" s="238"/>
-      <c r="D36" s="238"/>
-      <c r="E36" s="238"/>
-      <c r="F36" s="238"/>
-      <c r="G36" s="238"/>
-      <c r="H36" s="238"/>
-      <c r="I36" s="238"/>
+      <c r="B36" s="250"/>
+      <c r="C36" s="250"/>
+      <c r="D36" s="250"/>
+      <c r="E36" s="250"/>
+      <c r="F36" s="250"/>
+      <c r="G36" s="250"/>
+      <c r="H36" s="250"/>
+      <c r="I36" s="250"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="207" t="s">
@@ -22526,12 +22555,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="239" t="s">
+      <c r="A46" s="257" t="s">
         <v>318</v>
       </c>
-      <c r="B46" s="239"/>
-      <c r="C46" s="239"/>
-      <c r="D46" s="239"/>
+      <c r="B46" s="257"/>
+      <c r="C46" s="257"/>
+      <c r="D46" s="257"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="207" t="s">
@@ -22633,7 +22662,7 @@
       <c r="C52" s="123">
         <v>0.5</v>
       </c>
-      <c r="D52" s="282">
+      <c r="D52" s="227">
         <f>2*((B52*C52)/(B52+C52))</f>
         <v>8.2063521204332662E-2</v>
       </c>
@@ -22682,6 +22711,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -22690,18 +22727,10 @@
     <mergeCell ref="D6:D13"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="D27:G27"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="A17:G17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22713,8 +22742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22729,17 +22758,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="254" t="s">
+      <c r="A1" s="261" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
+      <c r="B1" s="262"/>
+      <c r="C1" s="262"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="262"/>
+      <c r="I1" s="262"/>
     </row>
     <row r="2" spans="1:19" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="220" t="s">
@@ -22755,30 +22784,30 @@
       <c r="I2" s="219"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="250" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="238"/>
-      <c r="C3" s="238"/>
-      <c r="D3" s="238"/>
-      <c r="E3" s="238"/>
-      <c r="F3" s="238"/>
-      <c r="G3" s="238"/>
-      <c r="H3" s="238"/>
-      <c r="I3" s="238"/>
+      <c r="B3" s="250"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="250"/>
+      <c r="E3" s="250"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="250"/>
+      <c r="I3" s="250"/>
     </row>
     <row r="4" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="243" t="s">
+      <c r="A4" s="251" t="s">
         <v>337</v>
       </c>
-      <c r="B4" s="243"/>
-      <c r="C4" s="243"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="243"/>
-      <c r="F4" s="243"/>
-      <c r="G4" s="243"/>
-      <c r="H4" s="243"/>
-      <c r="I4" s="243"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
       <c r="J4" s="70"/>
       <c r="K4" s="70"/>
       <c r="L4" s="70"/>
@@ -22791,15 +22820,15 @@
       <c r="S4" s="70"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="256" t="s">
+      <c r="A5" s="263" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="256"/>
-      <c r="C5" s="256"/>
-      <c r="D5" s="256"/>
-      <c r="E5" s="256"/>
-      <c r="F5" s="256"/>
-      <c r="G5" s="256"/>
+      <c r="B5" s="263"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
+      <c r="G5" s="263"/>
     </row>
     <row r="6" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="217" t="s">
@@ -22831,20 +22860,20 @@
       <c r="B7" s="49" t="s">
         <v>578</v>
       </c>
-      <c r="C7" s="278">
+      <c r="C7" s="223">
         <v>0.46666666666666701</v>
       </c>
       <c r="D7" s="49" t="s">
         <v>587</v>
       </c>
-      <c r="E7" s="278">
+      <c r="E7" s="223">
         <v>0.31818181818181801</v>
       </c>
-      <c r="F7" s="280">
+      <c r="F7" s="225">
         <f>HARMEAN(C7,E7)</f>
         <v>0.37837837837837834</v>
       </c>
-      <c r="G7" s="251" t="s">
+      <c r="G7" s="253" t="s">
         <v>339</v>
       </c>
       <c r="N7" s="26"/>
@@ -22856,20 +22885,20 @@
       <c r="B8" s="49" t="s">
         <v>579</v>
       </c>
-      <c r="C8" s="278">
+      <c r="C8" s="223">
         <v>1.41843971631206E-2</v>
       </c>
       <c r="D8" s="49" t="s">
         <v>580</v>
       </c>
-      <c r="E8" s="278">
+      <c r="E8" s="223">
         <v>9.0909090909090898E-2</v>
       </c>
-      <c r="F8" s="279">
+      <c r="F8" s="224">
         <f t="shared" ref="F8:F14" si="0">HARMEAN(C8,E8)</f>
         <v>2.4539877300613543E-2</v>
       </c>
-      <c r="G8" s="252"/>
+      <c r="G8" s="254"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
@@ -22878,20 +22907,20 @@
       <c r="B9" s="49" t="s">
         <v>581</v>
       </c>
-      <c r="C9" s="278">
+      <c r="C9" s="223">
         <v>0.38461538461538503</v>
       </c>
       <c r="D9" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="E9" s="278">
+      <c r="E9" s="223">
         <v>0.22727272727272699</v>
       </c>
-      <c r="F9" s="279">
+      <c r="F9" s="224">
         <f t="shared" si="0"/>
         <v>0.28571428571428559</v>
       </c>
-      <c r="G9" s="252"/>
+      <c r="G9" s="254"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
@@ -22900,20 +22929,20 @@
       <c r="B10" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="278">
+      <c r="C10" s="223">
         <v>0.5</v>
       </c>
       <c r="D10" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="E10" s="278">
+      <c r="E10" s="223">
         <v>0.22727272727272699</v>
       </c>
-      <c r="F10" s="279">
+      <c r="F10" s="224">
         <f t="shared" si="0"/>
         <v>0.31249999999999972</v>
       </c>
-      <c r="G10" s="252"/>
+      <c r="G10" s="254"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
@@ -22922,20 +22951,20 @@
       <c r="B11" s="49" t="s">
         <v>582</v>
       </c>
-      <c r="C11" s="278">
+      <c r="C11" s="223">
         <v>5.1282051282051299E-3</v>
       </c>
       <c r="D11" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="E11" s="278">
+      <c r="E11" s="223">
         <v>4.5454545454545497E-2</v>
       </c>
-      <c r="F11" s="279">
+      <c r="F11" s="224">
         <f t="shared" si="0"/>
         <v>9.2165898617511555E-3</v>
       </c>
-      <c r="G11" s="252"/>
+      <c r="G11" s="254"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
@@ -22944,20 +22973,20 @@
       <c r="B12" s="49" t="s">
         <v>583</v>
       </c>
-      <c r="C12" s="278">
+      <c r="C12" s="223">
         <v>0.05</v>
       </c>
       <c r="D12" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="E12" s="278">
+      <c r="E12" s="223">
         <v>0.22727272727272699</v>
       </c>
-      <c r="F12" s="279">
+      <c r="F12" s="224">
         <f t="shared" si="0"/>
         <v>8.1967213114754078E-2</v>
       </c>
-      <c r="G12" s="252"/>
+      <c r="G12" s="254"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
@@ -22966,42 +22995,42 @@
       <c r="B13" s="49" t="s">
         <v>584</v>
       </c>
-      <c r="C13" s="278">
+      <c r="C13" s="223">
         <v>0.13953488372093001</v>
       </c>
       <c r="D13" s="49" t="s">
         <v>585</v>
       </c>
-      <c r="E13" s="278">
+      <c r="E13" s="223">
         <v>0.27272727272727298</v>
       </c>
-      <c r="F13" s="279">
+      <c r="F13" s="224">
         <f t="shared" si="0"/>
         <v>0.18461538461538446</v>
       </c>
-      <c r="G13" s="252"/>
+      <c r="G13" s="254"/>
     </row>
     <row r="14" spans="1:19" s="76" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="141" t="s">
         <v>274</v>
       </c>
-      <c r="B14" s="277" t="s">
+      <c r="B14" s="222" t="s">
         <v>272</v>
       </c>
-      <c r="C14" s="278">
+      <c r="C14" s="223">
         <v>0.1</v>
       </c>
-      <c r="D14" s="277" t="s">
+      <c r="D14" s="222" t="s">
         <v>273</v>
       </c>
-      <c r="E14" s="278">
+      <c r="E14" s="223">
         <v>0.18181818181818199</v>
       </c>
-      <c r="F14" s="279">
+      <c r="F14" s="224">
         <f t="shared" si="0"/>
         <v>0.12903225806451618</v>
       </c>
-      <c r="G14" s="253"/>
+      <c r="G14" s="255"/>
     </row>
     <row r="15" spans="1:19" s="76" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="142" t="s">
@@ -23010,16 +23039,16 @@
       <c r="B15" s="91" t="s">
         <v>586</v>
       </c>
-      <c r="C15" s="278">
+      <c r="C15" s="223">
         <v>4.4265593561368201E-2</v>
       </c>
       <c r="D15" s="91" t="s">
         <v>588</v>
       </c>
-      <c r="E15" s="278">
+      <c r="E15" s="223">
         <v>0.43</v>
       </c>
-      <c r="F15" s="279">
+      <c r="F15" s="224">
         <f>HARMEAN(C15,E15)</f>
         <v>8.026812608714097E-2</v>
       </c>
@@ -23028,30 +23057,30 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="238" t="s">
+      <c r="A16" s="250" t="s">
         <v>261</v>
       </c>
-      <c r="B16" s="238"/>
-      <c r="C16" s="238"/>
-      <c r="D16" s="238"/>
-      <c r="E16" s="238"/>
-      <c r="F16" s="238"/>
-      <c r="G16" s="238"/>
-      <c r="H16" s="238"/>
-      <c r="I16" s="238"/>
+      <c r="B16" s="250"/>
+      <c r="C16" s="250"/>
+      <c r="D16" s="250"/>
+      <c r="E16" s="250"/>
+      <c r="F16" s="250"/>
+      <c r="G16" s="250"/>
+      <c r="H16" s="250"/>
+      <c r="I16" s="250"/>
     </row>
     <row r="17" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="243" t="s">
+      <c r="A17" s="251" t="s">
         <v>238</v>
       </c>
-      <c r="B17" s="243"/>
-      <c r="C17" s="243"/>
-      <c r="D17" s="243"/>
-      <c r="E17" s="243"/>
-      <c r="F17" s="243"/>
-      <c r="G17" s="243"/>
-      <c r="H17" s="243"/>
-      <c r="I17" s="243"/>
+      <c r="B17" s="251"/>
+      <c r="C17" s="251"/>
+      <c r="D17" s="251"/>
+      <c r="E17" s="251"/>
+      <c r="F17" s="251"/>
+      <c r="G17" s="251"/>
+      <c r="H17" s="251"/>
+      <c r="I17" s="251"/>
       <c r="J17" s="70"/>
       <c r="K17" s="70"/>
       <c r="L17" s="70"/>
@@ -23064,15 +23093,15 @@
       <c r="S17" s="70"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="256" t="s">
+      <c r="A18" s="263" t="s">
         <v>259</v>
       </c>
-      <c r="B18" s="256"/>
-      <c r="C18" s="256"/>
-      <c r="D18" s="256"/>
-      <c r="E18" s="256"/>
-      <c r="F18" s="256"/>
-      <c r="G18" s="256"/>
+      <c r="B18" s="263"/>
+      <c r="C18" s="263"/>
+      <c r="D18" s="263"/>
+      <c r="E18" s="263"/>
+      <c r="F18" s="263"/>
+      <c r="G18" s="263"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="217" t="s">
@@ -23116,7 +23145,7 @@
       <c r="F20" s="71">
         <v>1</v>
       </c>
-      <c r="G20" s="281">
+      <c r="G20" s="226">
         <f>HARMEAN(E20,F20)</f>
         <v>5.2959501557632398E-2</v>
       </c>
@@ -23140,7 +23169,7 @@
       <c r="F21" s="71">
         <v>0.70579999999999998</v>
       </c>
-      <c r="G21" s="281">
+      <c r="G21" s="226">
         <f t="shared" ref="G21:G25" si="1">HARMEAN(E21,F21)</f>
         <v>6.4692767338110038E-2</v>
       </c>
@@ -23164,7 +23193,7 @@
       <c r="F22" s="71">
         <v>0.86270000000000002</v>
       </c>
-      <c r="G22" s="281">
+      <c r="G22" s="226">
         <f t="shared" si="1"/>
         <v>7.1691989778913473E-2</v>
       </c>
@@ -23188,7 +23217,7 @@
       <c r="F23" s="71">
         <v>0.3725</v>
       </c>
-      <c r="G23" s="281">
+      <c r="G23" s="226">
         <f t="shared" si="1"/>
         <v>0.11068571428571429</v>
       </c>
@@ -23212,7 +23241,7 @@
       <c r="F24" s="71">
         <v>0.68620000000000003</v>
       </c>
-      <c r="G24" s="281">
+      <c r="G24" s="226">
         <f t="shared" si="1"/>
         <v>0.11355642293810987</v>
       </c>
@@ -23236,36 +23265,36 @@
       <c r="F25" s="71">
         <v>0.47049999999999997</v>
       </c>
-      <c r="G25" s="281">
+      <c r="G25" s="226">
         <f t="shared" si="1"/>
         <v>0.10342811199394626</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="238" t="s">
+      <c r="A26" s="250" t="s">
         <v>260</v>
       </c>
-      <c r="B26" s="238"/>
-      <c r="C26" s="238"/>
-      <c r="D26" s="238"/>
-      <c r="E26" s="238"/>
-      <c r="F26" s="238"/>
-      <c r="G26" s="238"/>
-      <c r="H26" s="238"/>
-      <c r="I26" s="238"/>
+      <c r="B26" s="250"/>
+      <c r="C26" s="250"/>
+      <c r="D26" s="250"/>
+      <c r="E26" s="250"/>
+      <c r="F26" s="250"/>
+      <c r="G26" s="250"/>
+      <c r="H26" s="250"/>
+      <c r="I26" s="250"/>
     </row>
     <row r="27" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="243" t="s">
+      <c r="A27" s="251" t="s">
         <v>338</v>
       </c>
-      <c r="B27" s="243"/>
-      <c r="C27" s="243"/>
-      <c r="D27" s="243"/>
-      <c r="E27" s="243"/>
-      <c r="F27" s="243"/>
-      <c r="G27" s="243"/>
-      <c r="H27" s="243"/>
-      <c r="I27" s="243"/>
+      <c r="B27" s="251"/>
+      <c r="C27" s="251"/>
+      <c r="D27" s="251"/>
+      <c r="E27" s="251"/>
+      <c r="F27" s="251"/>
+      <c r="G27" s="251"/>
+      <c r="H27" s="251"/>
+      <c r="I27" s="251"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="217" t="s">
@@ -23280,12 +23309,12 @@
       <c r="D28" s="218" t="s">
         <v>316</v>
       </c>
-      <c r="E28" s="283" t="s">
+      <c r="E28" s="264" t="s">
         <v>292</v>
       </c>
-      <c r="F28" s="284"/>
-      <c r="G28" s="284"/>
-      <c r="H28" s="285"/>
+      <c r="F28" s="265"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="266"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
@@ -23449,17 +23478,17 @@
       <c r="H35" s="210"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="238" t="s">
+      <c r="A37" s="250" t="s">
         <v>315</v>
       </c>
-      <c r="B37" s="238"/>
-      <c r="C37" s="238"/>
-      <c r="D37" s="238"/>
-      <c r="E37" s="238"/>
-      <c r="F37" s="238"/>
-      <c r="G37" s="238"/>
-      <c r="H37" s="238"/>
-      <c r="I37" s="238"/>
+      <c r="B37" s="250"/>
+      <c r="C37" s="250"/>
+      <c r="D37" s="250"/>
+      <c r="E37" s="250"/>
+      <c r="F37" s="250"/>
+      <c r="G37" s="250"/>
+      <c r="H37" s="250"/>
+      <c r="I37" s="250"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="217" t="s">
@@ -23550,8 +23579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23570,15 +23599,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="271" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="154" t="s">
@@ -23602,11 +23631,11 @@
       <c r="G2" s="154" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="256" t="s">
+      <c r="I2" s="263" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -24059,20 +24088,20 @@
       <c r="J22" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="262" t="s">
+      <c r="K22" s="272" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="262"/>
-      <c r="M22" s="262"/>
-      <c r="N22" s="262"/>
-      <c r="O22" s="262"/>
-      <c r="P22" s="262"/>
-      <c r="Q22" s="262"/>
-      <c r="R22" s="262"/>
-      <c r="S22" s="262"/>
-      <c r="T22" s="262"/>
-      <c r="U22" s="262"/>
-      <c r="V22" s="262"/>
+      <c r="L22" s="272"/>
+      <c r="M22" s="272"/>
+      <c r="N22" s="272"/>
+      <c r="O22" s="272"/>
+      <c r="P22" s="272"/>
+      <c r="Q22" s="272"/>
+      <c r="R22" s="272"/>
+      <c r="S22" s="272"/>
+      <c r="T22" s="272"/>
+      <c r="U22" s="272"/>
+      <c r="V22" s="272"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -24178,10 +24207,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="264"/>
-      <c r="B29" s="265"/>
-      <c r="C29" s="265"/>
-      <c r="D29" s="266"/>
+      <c r="A29" s="274"/>
+      <c r="B29" s="275"/>
+      <c r="C29" s="275"/>
+      <c r="D29" s="276"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -24198,10 +24227,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="267" t="s">
+      <c r="A31" s="277" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="268"/>
+      <c r="B31" s="278"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -24223,20 +24252,20 @@
       <c r="J32" s="113" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="263" t="s">
+      <c r="K32" s="273" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="263"/>
-      <c r="M32" s="263"/>
-      <c r="N32" s="263"/>
-      <c r="O32" s="263"/>
-      <c r="P32" s="263"/>
-      <c r="Q32" s="263"/>
-      <c r="R32" s="263"/>
-      <c r="S32" s="263"/>
-      <c r="T32" s="263"/>
-      <c r="U32" s="263"/>
-      <c r="V32" s="263"/>
+      <c r="L32" s="273"/>
+      <c r="M32" s="273"/>
+      <c r="N32" s="273"/>
+      <c r="O32" s="273"/>
+      <c r="P32" s="273"/>
+      <c r="Q32" s="273"/>
+      <c r="R32" s="273"/>
+      <c r="S32" s="273"/>
+      <c r="T32" s="273"/>
+      <c r="U32" s="273"/>
+      <c r="V32" s="273"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="83" t="s">
@@ -24269,10 +24298,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="257" t="s">
+      <c r="A35" s="267" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="259" t="s">
+      <c r="B35" s="269" t="s">
         <v>219</v>
       </c>
       <c r="D35" s="87"/>
@@ -24282,8 +24311,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="258"/>
-      <c r="B36" s="260"/>
+      <c r="A36" s="268"/>
+      <c r="B36" s="270"/>
       <c r="D36" s="87"/>
       <c r="I36" s="102" t="s">
         <v>296</v>
@@ -24377,7 +24406,7 @@
   <dimension ref="A1:V48"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24402,15 +24431,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="271" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="261"/>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="261"/>
-      <c r="G1" s="261"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
     </row>
     <row r="2" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="154" t="s">
@@ -24434,11 +24463,11 @@
       <c r="G2" s="154" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="256" t="s">
+      <c r="I2" s="263" t="s">
         <v>197</v>
       </c>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
       <c r="O2" s="166" t="s">
         <v>351</v>
       </c>
@@ -24939,20 +24968,20 @@
       <c r="J22" s="112" t="s">
         <v>217</v>
       </c>
-      <c r="K22" s="262" t="s">
+      <c r="K22" s="272" t="s">
         <v>307</v>
       </c>
-      <c r="L22" s="262"/>
-      <c r="M22" s="262"/>
-      <c r="N22" s="262"/>
-      <c r="O22" s="262"/>
-      <c r="P22" s="262"/>
-      <c r="Q22" s="262"/>
-      <c r="R22" s="262"/>
-      <c r="S22" s="262"/>
-      <c r="T22" s="262"/>
-      <c r="U22" s="262"/>
-      <c r="V22" s="262"/>
+      <c r="L22" s="272"/>
+      <c r="M22" s="272"/>
+      <c r="N22" s="272"/>
+      <c r="O22" s="272"/>
+      <c r="P22" s="272"/>
+      <c r="Q22" s="272"/>
+      <c r="R22" s="272"/>
+      <c r="S22" s="272"/>
+      <c r="T22" s="272"/>
+      <c r="U22" s="272"/>
+      <c r="V22" s="272"/>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
@@ -25058,10 +25087,10 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="264"/>
-      <c r="B29" s="265"/>
-      <c r="C29" s="265"/>
-      <c r="D29" s="266"/>
+      <c r="A29" s="274"/>
+      <c r="B29" s="275"/>
+      <c r="C29" s="275"/>
+      <c r="D29" s="276"/>
       <c r="I29" s="43" t="s">
         <v>187</v>
       </c>
@@ -25078,10 +25107,10 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="267" t="s">
+      <c r="A31" s="277" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="268"/>
+      <c r="B31" s="278"/>
       <c r="C31" s="68"/>
       <c r="I31" s="43" t="s">
         <v>189</v>
@@ -25103,20 +25132,20 @@
       <c r="J32" s="113" t="s">
         <v>308</v>
       </c>
-      <c r="K32" s="263" t="s">
+      <c r="K32" s="273" t="s">
         <v>306</v>
       </c>
-      <c r="L32" s="263"/>
-      <c r="M32" s="263"/>
-      <c r="N32" s="263"/>
-      <c r="O32" s="263"/>
-      <c r="P32" s="263"/>
-      <c r="Q32" s="263"/>
-      <c r="R32" s="263"/>
-      <c r="S32" s="263"/>
-      <c r="T32" s="263"/>
-      <c r="U32" s="263"/>
-      <c r="V32" s="263"/>
+      <c r="L32" s="273"/>
+      <c r="M32" s="273"/>
+      <c r="N32" s="273"/>
+      <c r="O32" s="273"/>
+      <c r="P32" s="273"/>
+      <c r="Q32" s="273"/>
+      <c r="R32" s="273"/>
+      <c r="S32" s="273"/>
+      <c r="T32" s="273"/>
+      <c r="U32" s="273"/>
+      <c r="V32" s="273"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="83" t="s">
@@ -25147,10 +25176,10 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="257" t="s">
+      <c r="A35" s="267" t="s">
         <v>184</v>
       </c>
-      <c r="B35" s="259" t="s">
+      <c r="B35" s="269" t="s">
         <v>219</v>
       </c>
       <c r="I35" s="43" t="s">
@@ -25159,8 +25188,8 @@
       <c r="J35" s="41"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="258"/>
-      <c r="B36" s="260"/>
+      <c r="A36" s="268"/>
+      <c r="B36" s="270"/>
       <c r="I36" s="102" t="s">
         <v>296</v>
       </c>

</xml_diff>